<commit_message>
Heavy work on paper. Running test on additionally trained memory sets.
</commit_message>
<xml_diff>
--- a/app/src/main/scala/testing/Tests/_TEST_RESULTS/Run_1/Experiment2/ChangeGoal-FHtoMW.xlsx
+++ b/app/src/main/scala/testing/Tests/_TEST_RESULTS/Run_1/Experiment2/ChangeGoal-FHtoMW.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3EB8A8-6265-494D-BF96-50144C9D9B8B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD43E02F-F384-4075-9B14-B3AFA64D64C4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EASY" sheetId="1" r:id="rId1"/>
@@ -14163,13 +14163,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>172402</xdr:colOff>
+      <xdr:colOff>75247</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>124777</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1180147</xdr:colOff>
+      <xdr:colOff>1086802</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>151447</xdr:rowOff>
     </xdr:to>
@@ -14199,15 +14199,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1524952</xdr:colOff>
+      <xdr:colOff>1086802</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>143827</xdr:rowOff>
+      <xdr:rowOff>124777</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>229552</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>429577</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>172402</xdr:rowOff>
+      <xdr:rowOff>151447</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14235,15 +14235,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>239077</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>162877</xdr:rowOff>
+      <xdr:colOff>77152</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>151447</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1248727</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>10477</xdr:rowOff>
+      <xdr:colOff>1086802</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>952</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14271,15 +14271,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1496377</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>115252</xdr:rowOff>
+      <xdr:colOff>1086802</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>151447</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>200977</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>427672</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>143827</xdr:rowOff>
+      <xdr:rowOff>952</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15032,8 +15032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0FB609-E3C8-4F28-A535-5E68054C2D4E}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Finished writting. Working on revisions.
</commit_message>
<xml_diff>
--- a/app/src/main/scala/testing/Tests/_TEST_RESULTS/Run_1/Experiment2/ChangeGoal-FHtoMW.xlsx
+++ b/app/src/main/scala/testing/Tests/_TEST_RESULTS/Run_1/Experiment2/ChangeGoal-FHtoMW.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD43E02F-F384-4075-9B14-B3AFA64D64C4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46C228C-A637-40DB-8FE6-6FBD1E576744}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EASY" sheetId="1" r:id="rId1"/>
@@ -1366,6 +1366,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Average Goal Completion (%)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1379,7 +1404,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1426,6 +1451,63 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-8A83-4102-843A-44CB1B39C2D8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-8A83-4102-843A-44CB1B39C2D8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-8A83-4102-843A-44CB1B39C2D8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>Overall!$I$2:$I$7</c:f>
@@ -1527,7 +1609,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1672,6 +1754,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Average Actions Performed (number of actions)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1685,7 +1792,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1732,6 +1839,63 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-C7FE-47D0-8A18-1C0574FEBB69}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-C7FE-47D0-8A18-1C0574FEBB69}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-C7FE-47D0-8A18-1C0574FEBB69}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>Overall!$I$2:$I$7</c:f>
@@ -1833,7 +1997,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1978,6 +2142,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Average Remaining Health (%)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1991,7 +2180,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2038,6 +2227,63 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-6416-4AF8-B8CB-A644772115B8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-6416-4AF8-B8CB-A644772115B8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-6416-4AF8-B8CB-A644772115B8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>Overall!$I$2:$I$7</c:f>
@@ -2139,7 +2385,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2284,6 +2530,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Average Remaining Energy (%)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2297,7 +2568,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2344,6 +2615,63 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-3C3F-4ABD-A32F-FE9A786178AC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-3C3F-4ABD-A32F-FE9A786178AC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-3C3F-4ABD-A32F-FE9A786178AC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>Overall!$I$2:$I$7</c:f>
@@ -2445,7 +2773,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -15032,8 +15360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0FB609-E3C8-4F28-A535-5E68054C2D4E}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X38" sqref="X38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>